<commit_message>
added rigid 10k to print settings
</commit_message>
<xml_diff>
--- a/settings/settings_printers_cutters.xlsx
+++ b/settings/settings_printers_cutters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scvro\Documents\GitHub\3D-scan-to-print\settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siets\Documents\Github\3D-scan-to-print\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3E5D40-5064-4CD7-A07B-3B9D74C1D1F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBA5ACE-B46D-4005-91A7-4A46B4D5BC0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{6D5578FB-A4FD-4854-B90C-034445EFB167}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D5578FB-A4FD-4854-B90C-034445EFB167}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Printing with:</t>
   </si>
@@ -209,6 +209,33 @@
   </si>
   <si>
     <t>Use Resin Tank LT(Form 2) or Resin Tank V2 (Form 3) are required for printing with Rigid 10K Resin when printing with Rigid 10K Resin. Standard resin tanks are incompatible with Rigid 10K Resin because the elastic layer in a standard resin tank swells when exposed to the uncured material.</t>
+  </si>
+  <si>
+    <t>materials</t>
+  </si>
+  <si>
+    <t>curing time</t>
+  </si>
+  <si>
+    <t>rigid 10K V1</t>
+  </si>
+  <si>
+    <t>curing temp</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>70 °C</t>
+  </si>
+  <si>
+    <t>Optionally, post-cure and then heat the printed part at 125 ºC for 90 minutes for a higher heat deflection temperature.</t>
+  </si>
+  <si>
+    <t>~</t>
   </si>
 </sst>
 </file>
@@ -260,15 +287,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -410,12 +443,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -481,6 +549,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -796,27 +890,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147EBECA-DB97-4218-82D4-5E82205B7327}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5234375" customWidth="1"/>
-    <col min="2" max="2" width="18.3125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="18.3125" style="6" customWidth="1"/>
-    <col min="5" max="8" width="17.41796875" customWidth="1"/>
-    <col min="9" max="10" width="17.41796875" style="14" customWidth="1"/>
-    <col min="11" max="11" width="18.1015625" customWidth="1"/>
-    <col min="12" max="12" width="12.41796875" customWidth="1"/>
-    <col min="13" max="13" width="12.3125" customWidth="1"/>
-    <col min="14" max="14" width="12.20703125" customWidth="1"/>
-    <col min="16" max="16" width="15.68359375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="51" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" style="51" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" style="14" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.21875" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -829,28 +931,36 @@
       <c r="E1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="47"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="47"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E2" s="30"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" s="48"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="55"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -863,23 +973,27 @@
       <c r="E3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="K3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13" t="s">
+      <c r="L3" s="48"/>
+      <c r="M3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="N3" s="10"/>
+      <c r="O3" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="25"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3" s="25"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -892,29 +1006,37 @@
       <c r="E4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="F4" s="48"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="N4" s="10"/>
+      <c r="O4" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="25"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="P4" s="25"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E5" s="30"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L5" s="48"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
@@ -927,65 +1049,84 @@
       <c r="E6" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25" t="s">
+      <c r="F6" s="48"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="K6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="48"/>
+      <c r="M6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="O6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="P6" s="25"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="34"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
       <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L7" s="48"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E8" s="30"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L8" s="48"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E9" s="30"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
       <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-    </row>
-    <row r="10" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="L9" s="48"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+    </row>
+    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="E10" s="29"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L10" s="47"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -998,15 +1139,19 @@
       <c r="E11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="L11" s="48"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1019,133 +1164,205 @@
       <c r="E12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L12" s="47"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
       <c r="E13" s="30"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="34"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L13" s="48"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="9"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="48"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L15" s="48"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E16" s="30"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="48"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="48"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="30"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="48"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="48"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E18" s="30"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="48"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="48"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="30"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="L19" s="48"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="30"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="L20" s="48"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+    </row>
+    <row r="21" spans="1:16" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="33"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
       <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="L21" s="49"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="1:16" s="5" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="33"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="28" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" s="49"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>18</v>
       </c>
@@ -1155,10 +1372,13 @@
       <c r="C28" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="F28" s="50"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="1"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="18"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C29" s="6" t="s">
         <v>17</v>
       </c>
@@ -1166,7 +1386,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C30" s="6" t="s">
         <v>15</v>
       </c>
@@ -1174,10 +1394,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
@@ -1186,7 +1406,7 @@
       </c>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C33" s="6" t="s">
         <v>17</v>
       </c>
@@ -1194,7 +1414,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C34" s="6" t="s">
         <v>15</v>
       </c>
@@ -1202,10 +1422,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>21</v>
       </c>
@@ -1214,7 +1434,7 @@
       </c>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C37" s="6" t="s">
         <v>17</v>
       </c>
@@ -1222,20 +1442,24 @@
         <v>605</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D38">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="19"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="F39" s="52"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="2"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="21"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1246,7 +1470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C41" s="6" t="s">
         <v>17</v>
       </c>
@@ -1254,7 +1478,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1262,7 +1486,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>20</v>
       </c>
@@ -1270,17 +1494,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C45" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C46" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>21</v>
       </c>
@@ -1288,7 +1512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C49" s="6" t="s">
         <v>17</v>
       </c>
@@ -1296,7 +1520,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="3" t="s">
         <v>15</v>
@@ -1304,8 +1528,11 @@
       <c r="D50" s="3">
         <v>80</v>
       </c>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="2"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,102 +1543,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8439C50E-456D-4392-879A-7DAA857A4E8B}">
   <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="152.7890625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="152.77734375" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:2" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="39"/>
     </row>
-    <row r="6" spans="2:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="39"/>
     </row>
-    <row r="8" spans="2:2" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:2" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="39"/>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" s="39"/>
     </row>
-    <row r="14" spans="2:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="39"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="39" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="39"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="39"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="39" t="s">
         <v>54</v>
       </c>

</xml_diff>